<commit_message>
Added Example Column in Mapping-Sheet and added cell-formatting
</commit_message>
<xml_diff>
--- a/Manual Tasks/WebTemplate_Datatypes_MAPPING.xlsx
+++ b/Manual Tasks/WebTemplate_Datatypes_MAPPING.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="200">
   <si>
     <t>FLAT-Path</t>
   </si>
@@ -350,6 +350,9 @@
     <t>Bei FLAT-Pfaden mit dem Element "&lt;&lt;index&gt;&gt;" wählen Sie den Index (z.B. für eine best. Messung) beginnend mit 0</t>
   </si>
   <si>
+    <t>context_start_time/value</t>
+  </si>
+  <si>
     <t>EHRID</t>
   </si>
   <si>
@@ -368,85 +371,250 @@
     <t>Endzeit</t>
   </si>
   <si>
-    <t>BemerkungenAssessment/value</t>
-  </si>
-  <si>
-    <t>Profane_Sturz/symbol/defining_code/code_string</t>
-  </si>
-  <si>
-    <t>Profane_Sturz/symbol/defining_code/terminology_id/value</t>
-  </si>
-  <si>
-    <t>Profane_Sturz/symbol/value</t>
-  </si>
-  <si>
-    <t>Profane_Sturz/value</t>
-  </si>
-  <si>
-    <t>Profane_HaeufigkeitSturz/magnitude</t>
-  </si>
-  <si>
-    <t>Profane_ZeitSturz/value</t>
-  </si>
-  <si>
-    <t>Profane_VerletzungErlitten/symbol/defining_code/code_string</t>
-  </si>
-  <si>
-    <t>Profane_VerletzungErlitten/symbol/defining_code/terminology_id/value</t>
-  </si>
-  <si>
-    <t>Profane_VerletzungErlitten/symbol/value</t>
-  </si>
-  <si>
-    <t>Profane_VerletzungErlitten/value</t>
-  </si>
-  <si>
-    <t>Profane_Bruch/symbol/defining_code/code_string</t>
-  </si>
-  <si>
-    <t>Profane_Bruch/symbol/defining_code/terminology_id/value</t>
-  </si>
-  <si>
-    <t>Profane_Bruch/symbol/value</t>
-  </si>
-  <si>
-    <t>Profane_Bruch/value</t>
-  </si>
-  <si>
-    <t>Profane_LokalisationBruch/value</t>
-  </si>
-  <si>
-    <t>Profane_WeitereVerletzungen/value</t>
-  </si>
-  <si>
-    <t>Profane_Bemerkungen/value</t>
-  </si>
-  <si>
-    <t>Schmerz_SchmerzenVorhanden/value</t>
-  </si>
-  <si>
-    <t>Schmerz_Lokalisation/value</t>
-  </si>
-  <si>
-    <t>Schmerz_DauerVerlauf/value</t>
-  </si>
-  <si>
-    <t>Schmerz_VASSchmerzstaerke/magnitude</t>
-  </si>
-  <si>
-    <t>Unnamed: 28</t>
-  </si>
-  <si>
-    <t>Schmerz_VASBewegung/magnitude</t>
-  </si>
-  <si>
-    <t>Schmerz_VASBewegung/units</t>
-  </si>
-  <si>
-    <t>BMI/magnitude</t>
-  </si>
-  <si>
-    <t>BMI/units</t>
+    <t>Profane/archetype_details/archetype_id/value</t>
+  </si>
+  <si>
+    <t>Profane/archetype_details/rm_version</t>
+  </si>
+  <si>
+    <t>Profane/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Profane/Tree/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Kein Assessment vorhanden/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Kein Assessment vorhanden/name/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Kein Assessment vorhanden/value/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/name/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/value/symbol/defining_code/code_string</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/value/symbol/defining_code/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/value/symbol/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Grund/value/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/name/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/value/symbol/defining_code/code_string</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/value/symbol/defining_code/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/value/symbol/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/Sind Sie seit meinem letzten Besuch gest�rzt, ausgerutscht oder gestolpert, sodass Sie auf dem Boden zu liegen gekommen sind?/value/value</t>
+  </si>
+  <si>
+    <t>Profane/Tree/name/value</t>
+  </si>
+  <si>
+    <t>Profane/encoding/code_string</t>
+  </si>
+  <si>
+    <t>Profane/encoding/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Profane/language/code_string</t>
+  </si>
+  <si>
+    <t>Profane/language/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Profane/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/archetype_details/archetype_id/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/archetype_details/rm_version</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Kein Assessment vorhanden/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Kein Assessment vorhanden/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Kein Assessment vorhanden/value/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Haben Sie Schmerzen?/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Haben Sie Schmerzen?/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Haben Sie Schmerzen?/value/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wo?/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wo?/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wo?/value/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wie lange haben Sie die Schmerzen schon?/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wie lange haben Sie die Schmerzen schon?/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/Wie lange haben Sie die Schmerzen schon?/value/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzlokalisation/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzst�rke/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzst�rke/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzst�rke/value/magnitude</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Schmerzst�rke/value/units</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Bewegungseinschr�nkungen durch die Schmerzen/archetype_node_id</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Bewegungseinschr�nkungen durch die Schmerzen/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Bewegungseinschr�nkungen durch die Schmerzen/value/magnitude</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/Bewegungseinschr�nkungen durch die Schmerzen/value/units</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/Tree/name/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/encoding/code_string</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/encoding/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/language/code_string</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/language/terminology_id/value</t>
+  </si>
+  <si>
+    <t>Schmerzerfassung/name/value</t>
+  </si>
+  <si>
+    <t>BMI/archetype_details/archetype_id/value</t>
+  </si>
+  <si>
+    <t>BMI/archetype_details/rm_version</t>
+  </si>
+  <si>
+    <t>BMI/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Kein Assessment vorhanden/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Kein Assessment vorhanden/name/value</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Kein Assessment vorhanden/value/value</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Gewicht/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Gewicht/name/value</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Gewicht/value/magnitude</t>
+  </si>
+  <si>
+    <t>BMI/Tree/Gewicht/value/units</t>
+  </si>
+  <si>
+    <t>BMI/Tree/K�rpergr��e/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/K�rpergr��e/name/value</t>
+  </si>
+  <si>
+    <t>BMI/Tree/K�rpergr��e/value/magnitude</t>
+  </si>
+  <si>
+    <t>BMI/Tree/K�rpergr��e/value/units</t>
+  </si>
+  <si>
+    <t>BMI/Tree/BMI/archetype_node_id</t>
+  </si>
+  <si>
+    <t>BMI/Tree/BMI/name/value</t>
+  </si>
+  <si>
+    <t>BMI/Tree/BMI/value/magnitude</t>
+  </si>
+  <si>
+    <t>BMI/Tree/BMI/value/units</t>
+  </si>
+  <si>
+    <t>BMI/Tree/name/value</t>
+  </si>
+  <si>
+    <t>BMI/encoding/code_string</t>
+  </si>
+  <si>
+    <t>BMI/encoding/terminology_id/value</t>
+  </si>
+  <si>
+    <t>BMI/language/code_string</t>
+  </si>
+  <si>
+    <t>BMI/language/terminology_id/value</t>
+  </si>
+  <si>
+    <t>BMI/name/value</t>
   </si>
 </sst>
 </file>
@@ -778,7 +946,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -971,8 +1139,288 @@
         <v>143</v>
       </c>
     </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="33">
+  <dataValidations count="89">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>FLAT_Paths!$A$2:$A$87</formula1>
     </dataValidation>
@@ -1070,6 +1518,174 @@
       <formula1>FLAT_Paths!$A$2:$A$87</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
+      <formula1>FLAT_Paths!$A$2:$A$87</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90">
       <formula1>FLAT_Paths!$A$2:$A$87</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>